<commit_message>
修改了部分英雄姓名的特定显示【Modified Specific Champions' Name Display】
现在，维克兹、卑尔维斯和奎桑提的英文姓名将按照美服英雄联盟官网的英雄页面的格式显示。
Now, Vel'Koz's, Bel'Veth's and K'Sante's names are displayed according to the pattern in the "CHAMPIONS" page on NA LoL official website.
此外，维护了部分个人隐私信息。
Besides, hid some personal information.

未来规划（Future Prospects）：
新建一个自定义脚本，创建英雄联盟对局数据的二维表，用户在最后一列补充玩家的对局得分（OP分数、WeGame/掌上英雄联盟评分和游戏内荣誉评价）。当一个用户能积累上千场甚至上万场对局的数据时，就可以进行分数计算模型的预测。
Create a customized program that creates a two-dimension table about match data. Users add the scores (OP score, WeGame score or post-game honor grade) after the last column. If a user accumulates data of thousands matches, he can use these data to predict the calculation model of these scores.
</commit_message>
<xml_diff>
--- a/available-bots.xlsx
+++ b/available-bots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19250\Desktop\英雄联盟自定义房间创建\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14AB498-98A9-46F4-8F90-EBBE39F44C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE8B613-80C3-49F0-B50E-BC0E9B9D9B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{79371658-E0FE-43C3-8A19-9910316D4D47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{79371658-E0FE-43C3-8A19-9910316D4D47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,17 +38,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="335">
   <si>
     <t>championId</t>
   </si>
   <si>
-    <t>CN</t>
-  </si>
-  <si>
-    <t>EN</t>
-  </si>
-  <si>
     <t>黑暗之女</t>
   </si>
   <si>
@@ -214,9 +208,6 @@
     <t>齐天大圣</t>
   </si>
   <si>
-    <t>Wukong</t>
-  </si>
-  <si>
     <t>复仇焰魂</t>
   </si>
   <si>
@@ -316,726 +307,610 @@
     <t>Lucian</t>
   </si>
   <si>
+    <t>远古恐惧</t>
+  </si>
+  <si>
+    <t>雪原双子</t>
+  </si>
+  <si>
+    <t>Nunu &amp; Willump</t>
+  </si>
+  <si>
+    <t>蛮族之王</t>
+  </si>
+  <si>
+    <t>Tryndamere</t>
+  </si>
+  <si>
+    <t>炼金术士</t>
+  </si>
+  <si>
+    <t>Singed</t>
+  </si>
+  <si>
+    <t>Evelynn</t>
+  </si>
+  <si>
+    <t>瘟疫之源</t>
+  </si>
+  <si>
+    <t>Twitch</t>
+  </si>
+  <si>
+    <t>痛苦之拥</t>
+  </si>
+  <si>
+    <t>冰晶凤凰</t>
+  </si>
+  <si>
+    <t>恶魔小丑</t>
+  </si>
+  <si>
+    <t>Shaco</t>
+  </si>
+  <si>
+    <t>狂战士</t>
+  </si>
+  <si>
+    <t>卡牌大师</t>
+  </si>
+  <si>
+    <t>德邦总管</t>
+  </si>
+  <si>
+    <t>无畏战车</t>
+  </si>
+  <si>
+    <t>诡术妖姬</t>
+  </si>
+  <si>
+    <t>亡灵战神</t>
+  </si>
+  <si>
+    <t>迅捷斥候</t>
+  </si>
+  <si>
+    <t>琴瑟仙女</t>
+  </si>
+  <si>
+    <t>虚空行者</t>
+  </si>
+  <si>
+    <t>刀锋舞者</t>
+  </si>
+  <si>
+    <t>风暴之怒</t>
+  </si>
+  <si>
+    <t>海洋之灾</t>
+  </si>
+  <si>
+    <t>英勇投弹手</t>
+  </si>
+  <si>
+    <t>天启者</t>
+  </si>
+  <si>
+    <t>诺克萨斯统领</t>
+  </si>
+  <si>
+    <t>不祥之刃</t>
+  </si>
+  <si>
+    <t>永恒梦魇</t>
+  </si>
+  <si>
+    <t>扭曲树精</t>
+  </si>
+  <si>
+    <t>德玛西亚皇子</t>
+  </si>
+  <si>
+    <t>蜘蛛女皇</t>
+  </si>
+  <si>
+    <t>发条魔灵</t>
+  </si>
+  <si>
+    <t>盲僧</t>
+  </si>
+  <si>
+    <t>暗夜猎手</t>
+  </si>
+  <si>
+    <t>机械公敌</t>
+  </si>
+  <si>
+    <t>水晶先锋</t>
+  </si>
+  <si>
+    <t>大发明家</t>
+  </si>
+  <si>
+    <t>圣锤之毅</t>
+  </si>
+  <si>
+    <t>酒桶</t>
+  </si>
+  <si>
+    <t>不屈之枪</t>
+  </si>
+  <si>
+    <t>铁铠冥魂</t>
+  </si>
+  <si>
+    <t>牧魂人</t>
+  </si>
+  <si>
+    <t>离群之刺</t>
+  </si>
+  <si>
+    <t>狂暴之心</t>
+  </si>
+  <si>
+    <t>虚空先知</t>
+  </si>
+  <si>
+    <t>刀锋之影</t>
+  </si>
+  <si>
+    <t>放逐之刃</t>
+  </si>
+  <si>
+    <t>远古巫灵</t>
+  </si>
+  <si>
+    <t>九尾妖狐</t>
+  </si>
+  <si>
+    <t>潮汐海灵</t>
+  </si>
+  <si>
+    <t>不灭狂雷</t>
+  </si>
+  <si>
+    <t>傲之追猎者</t>
+  </si>
+  <si>
+    <t>惩戒之箭</t>
+  </si>
+  <si>
+    <t>深海泰坦</t>
+  </si>
+  <si>
+    <t>机械先驱</t>
+  </si>
+  <si>
+    <t>北地之怒</t>
+  </si>
+  <si>
+    <t>无双剑姬</t>
+  </si>
+  <si>
+    <t>仙灵女巫</t>
+  </si>
+  <si>
+    <t>荣耀行刑官</t>
+  </si>
+  <si>
+    <t>战争之影</t>
+  </si>
+  <si>
+    <t>虚空掠夺者</t>
+  </si>
+  <si>
+    <t>未来守护者</t>
+  </si>
+  <si>
+    <t>冰霜女巫</t>
+  </si>
+  <si>
+    <t>皎月女神</t>
+  </si>
+  <si>
+    <t>德玛西亚之翼</t>
+  </si>
+  <si>
+    <t>暗黑元首</t>
+  </si>
+  <si>
+    <t>铸星龙王</t>
+  </si>
+  <si>
+    <t>影流之镰</t>
+  </si>
+  <si>
+    <t>暮光星灵</t>
+  </si>
+  <si>
+    <t>虚空之女</t>
+  </si>
+  <si>
+    <t>星籁歌姬</t>
+  </si>
+  <si>
+    <t>迷失之牙</t>
+  </si>
+  <si>
+    <t>生化魔人</t>
+  </si>
+  <si>
+    <t>疾风剑豪</t>
+  </si>
+  <si>
+    <t>虚空之眼</t>
+  </si>
+  <si>
+    <t>岩雀</t>
+  </si>
+  <si>
+    <t>青钢影</t>
+  </si>
+  <si>
+    <t>影哨</t>
+  </si>
+  <si>
+    <t>弗雷尔卓德之心</t>
+  </si>
+  <si>
+    <t>戏命师</t>
+  </si>
+  <si>
+    <t>永猎双子</t>
+  </si>
+  <si>
+    <t>祖安花火</t>
+  </si>
+  <si>
+    <t>暴走萝莉</t>
+  </si>
+  <si>
+    <t>河流之王</t>
+  </si>
+  <si>
+    <t>破败之王</t>
+  </si>
+  <si>
+    <t>涤魂圣枪</t>
+  </si>
+  <si>
+    <t>影流之主</t>
+  </si>
+  <si>
+    <t>暴怒骑士</t>
+  </si>
+  <si>
+    <t>时间刺客</t>
+  </si>
+  <si>
+    <t>元素女皇</t>
+  </si>
+  <si>
+    <t>皮城执法官</t>
+  </si>
+  <si>
+    <t>暗裔剑魔</t>
+  </si>
+  <si>
+    <t>唤潮鲛姬</t>
+  </si>
+  <si>
+    <t>沙漠皇帝</t>
+  </si>
+  <si>
+    <t>魔法猫咪</t>
+  </si>
+  <si>
+    <t>沙漠玫瑰</t>
+  </si>
+  <si>
+    <t>魂锁典狱长</t>
+  </si>
+  <si>
+    <t>海兽祭司</t>
+  </si>
+  <si>
+    <t>虚空遁地兽</t>
+  </si>
+  <si>
+    <t>翠神</t>
+  </si>
+  <si>
+    <t>复仇之矛</t>
+  </si>
+  <si>
+    <t>星界游神</t>
+  </si>
+  <si>
+    <t>幻翎</t>
+  </si>
+  <si>
+    <t>逆羽</t>
+  </si>
+  <si>
+    <t>山隐之焰</t>
+  </si>
+  <si>
+    <t>解脱者</t>
+  </si>
+  <si>
+    <t>万花通灵</t>
+  </si>
+  <si>
+    <t>残月之肃</t>
+  </si>
+  <si>
+    <t>镕铁少女</t>
+  </si>
+  <si>
+    <t>血港鬼影</t>
+  </si>
+  <si>
+    <t>愁云使者</t>
+  </si>
+  <si>
+    <t>封魔剑魂</t>
+  </si>
+  <si>
+    <t>腕豪</t>
+  </si>
+  <si>
+    <t>含羞蓓蕾</t>
+  </si>
+  <si>
+    <t>灵罗娃娃</t>
+  </si>
+  <si>
+    <t>炼金男爵</t>
+  </si>
+  <si>
+    <t>Olaf</t>
+  </si>
+  <si>
+    <t>Twisted Fate</t>
+  </si>
+  <si>
+    <t>Xin Zhao</t>
+  </si>
+  <si>
+    <t>Urgot</t>
+  </si>
+  <si>
+    <t>Sion</t>
+  </si>
+  <si>
+    <t>Teemo</t>
+  </si>
+  <si>
     <t>Cho'Gath</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anivia</t>
   </si>
   <si>
     <t>Dr. Mundo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sona</t>
+  </si>
+  <si>
+    <t>Kassadin</t>
+  </si>
+  <si>
+    <t>Irelia</t>
+  </si>
+  <si>
+    <t>Janna</t>
+  </si>
+  <si>
+    <t>Gangplank</t>
+  </si>
+  <si>
+    <t>Corki</t>
+  </si>
+  <si>
+    <t>Karma</t>
+  </si>
+  <si>
+    <t>Swain</t>
+  </si>
+  <si>
+    <t>Katarina</t>
+  </si>
+  <si>
+    <t>Nocturne</t>
+  </si>
+  <si>
+    <t>Maokai</t>
+  </si>
+  <si>
+    <t>Jarvan IV</t>
+  </si>
+  <si>
+    <t>Elise</t>
+  </si>
+  <si>
+    <t>Orianna</t>
+  </si>
+  <si>
+    <t>Lee Sin</t>
+  </si>
+  <si>
+    <t>Vayne</t>
+  </si>
+  <si>
+    <t>Rumble</t>
+  </si>
+  <si>
+    <t>Skarner</t>
+  </si>
+  <si>
+    <t>Heimerdinger</t>
+  </si>
+  <si>
+    <t>Poppy</t>
+  </si>
+  <si>
+    <t>Gragas</t>
+  </si>
+  <si>
+    <t>Pantheon</t>
+  </si>
+  <si>
+    <t>Mordekaiser</t>
+  </si>
+  <si>
+    <t>Yorick</t>
+  </si>
+  <si>
+    <t>Akali</t>
+  </si>
+  <si>
+    <t>Kennen</t>
+  </si>
+  <si>
+    <t>Malzahar</t>
+  </si>
+  <si>
+    <t>Talon</t>
+  </si>
+  <si>
+    <t>Riven</t>
   </si>
   <si>
     <t>Kog'Maw</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Olaf</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Teemo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Katarina</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nocturne</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Orianna</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Vayne</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Heimerdinger</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Malzahar</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Xerath</t>
   </si>
   <si>
     <t>Ahri</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fizz</t>
+  </si>
+  <si>
+    <t>Volibear</t>
+  </si>
+  <si>
+    <t>Rengar</t>
+  </si>
+  <si>
+    <t>Varus</t>
+  </si>
+  <si>
+    <t>Nautilus</t>
+  </si>
+  <si>
+    <t>Viktor</t>
+  </si>
+  <si>
+    <t>Sejuani</t>
+  </si>
+  <si>
+    <t>Fiora</t>
   </si>
   <si>
     <t>Lulu</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Draven</t>
+  </si>
+  <si>
+    <t>Hecarim</t>
+  </si>
+  <si>
+    <t>Jayce</t>
+  </si>
+  <si>
+    <t>Lissandra</t>
+  </si>
+  <si>
+    <t>Diana</t>
+  </si>
+  <si>
+    <t>Quinn</t>
+  </si>
+  <si>
+    <t>Syndra</t>
+  </si>
+  <si>
+    <t>Aurelion Sol</t>
+  </si>
+  <si>
+    <t>Kayn</t>
+  </si>
+  <si>
+    <t>Zoe</t>
+  </si>
+  <si>
+    <t>Kai'Sa</t>
+  </si>
+  <si>
+    <t>Seraphine</t>
+  </si>
+  <si>
+    <t>Gnar</t>
+  </si>
+  <si>
+    <t>Zac</t>
+  </si>
+  <si>
+    <t>Yasuo</t>
+  </si>
+  <si>
+    <t>Taliyah</t>
+  </si>
+  <si>
+    <t>Camille</t>
+  </si>
+  <si>
+    <t>Akshan</t>
+  </si>
+  <si>
+    <t>Braum</t>
+  </si>
+  <si>
+    <t>Jhin</t>
+  </si>
+  <si>
+    <t>Kindred</t>
+  </si>
+  <si>
+    <t>Zeri</t>
   </si>
   <si>
     <t>Jinx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tahm Kench</t>
+  </si>
+  <si>
+    <t>Viego</t>
+  </si>
+  <si>
+    <t>Senna</t>
+  </si>
+  <si>
+    <t>Zed</t>
+  </si>
+  <si>
+    <t>Kled</t>
+  </si>
+  <si>
+    <t>Ekko</t>
+  </si>
+  <si>
+    <t>Qiyana</t>
+  </si>
+  <si>
+    <t>Vi</t>
+  </si>
+  <si>
+    <t>Aatrox</t>
   </si>
   <si>
     <t>Nami</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>狂战士</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>亡灵战神</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>不祥之刃</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>永恒梦魇</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>发条魔灵</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>暗夜猎手</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>大发明家</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>虚空先知</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>九尾妖狐</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>仙灵女巫</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>暴走萝莉</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>唤潮鲛姬</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>迅捷斥候</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>远古恐惧</t>
-  </si>
-  <si>
-    <t>雪原双子</t>
-  </si>
-  <si>
-    <t>Nunu &amp; Willump</t>
-  </si>
-  <si>
-    <t>蛮族之王</t>
-  </si>
-  <si>
-    <t>Tryndamere</t>
-  </si>
-  <si>
-    <t>炼金术士</t>
-  </si>
-  <si>
-    <t>Singed</t>
-  </si>
-  <si>
-    <t>Evelynn</t>
-  </si>
-  <si>
-    <t>瘟疫之源</t>
-  </si>
-  <si>
-    <t>Twitch</t>
-  </si>
-  <si>
-    <t>痛苦之拥</t>
-  </si>
-  <si>
-    <t>冰晶凤凰</t>
-  </si>
-  <si>
-    <t>恶魔小丑</t>
-  </si>
-  <si>
-    <t>Shaco</t>
-  </si>
-  <si>
-    <t>狂战士</t>
-  </si>
-  <si>
-    <t>卡牌大师</t>
-  </si>
-  <si>
-    <t>德邦总管</t>
-  </si>
-  <si>
-    <t>无畏战车</t>
-  </si>
-  <si>
-    <t>诡术妖姬</t>
-  </si>
-  <si>
-    <t>亡灵战神</t>
-  </si>
-  <si>
-    <t>迅捷斥候</t>
-  </si>
-  <si>
-    <t>琴瑟仙女</t>
-  </si>
-  <si>
-    <t>虚空行者</t>
-  </si>
-  <si>
-    <t>刀锋舞者</t>
-  </si>
-  <si>
-    <t>风暴之怒</t>
-  </si>
-  <si>
-    <t>海洋之灾</t>
-  </si>
-  <si>
-    <t>英勇投弹手</t>
-  </si>
-  <si>
-    <t>天启者</t>
-  </si>
-  <si>
-    <t>诺克萨斯统领</t>
-  </si>
-  <si>
-    <t>不祥之刃</t>
-  </si>
-  <si>
-    <t>永恒梦魇</t>
-  </si>
-  <si>
-    <t>扭曲树精</t>
-  </si>
-  <si>
-    <t>德玛西亚皇子</t>
-  </si>
-  <si>
-    <t>蜘蛛女皇</t>
-  </si>
-  <si>
-    <t>发条魔灵</t>
-  </si>
-  <si>
-    <t>盲僧</t>
-  </si>
-  <si>
-    <t>暗夜猎手</t>
-  </si>
-  <si>
-    <t>机械公敌</t>
-  </si>
-  <si>
-    <t>水晶先锋</t>
-  </si>
-  <si>
-    <t>大发明家</t>
-  </si>
-  <si>
-    <t>圣锤之毅</t>
-  </si>
-  <si>
-    <t>酒桶</t>
-  </si>
-  <si>
-    <t>不屈之枪</t>
-  </si>
-  <si>
-    <t>铁铠冥魂</t>
-  </si>
-  <si>
-    <t>牧魂人</t>
-  </si>
-  <si>
-    <t>离群之刺</t>
-  </si>
-  <si>
-    <t>狂暴之心</t>
-  </si>
-  <si>
-    <t>虚空先知</t>
-  </si>
-  <si>
-    <t>刀锋之影</t>
-  </si>
-  <si>
-    <t>放逐之刃</t>
-  </si>
-  <si>
-    <t>远古巫灵</t>
-  </si>
-  <si>
-    <t>九尾妖狐</t>
-  </si>
-  <si>
-    <t>潮汐海灵</t>
-  </si>
-  <si>
-    <t>不灭狂雷</t>
-  </si>
-  <si>
-    <t>傲之追猎者</t>
-  </si>
-  <si>
-    <t>惩戒之箭</t>
-  </si>
-  <si>
-    <t>深海泰坦</t>
-  </si>
-  <si>
-    <t>机械先驱</t>
-  </si>
-  <si>
-    <t>北地之怒</t>
-  </si>
-  <si>
-    <t>无双剑姬</t>
-  </si>
-  <si>
-    <t>仙灵女巫</t>
-  </si>
-  <si>
-    <t>荣耀行刑官</t>
-  </si>
-  <si>
-    <t>战争之影</t>
-  </si>
-  <si>
-    <t>虚空掠夺者</t>
-  </si>
-  <si>
-    <t>未来守护者</t>
-  </si>
-  <si>
-    <t>冰霜女巫</t>
-  </si>
-  <si>
-    <t>皎月女神</t>
-  </si>
-  <si>
-    <t>德玛西亚之翼</t>
-  </si>
-  <si>
-    <t>暗黑元首</t>
-  </si>
-  <si>
-    <t>铸星龙王</t>
-  </si>
-  <si>
-    <t>影流之镰</t>
-  </si>
-  <si>
-    <t>暮光星灵</t>
-  </si>
-  <si>
-    <t>虚空之女</t>
-  </si>
-  <si>
-    <t>星籁歌姬</t>
-  </si>
-  <si>
-    <t>迷失之牙</t>
-  </si>
-  <si>
-    <t>生化魔人</t>
-  </si>
-  <si>
-    <t>疾风剑豪</t>
-  </si>
-  <si>
-    <t>虚空之眼</t>
-  </si>
-  <si>
-    <t>岩雀</t>
-  </si>
-  <si>
-    <t>青钢影</t>
-  </si>
-  <si>
-    <t>影哨</t>
-  </si>
-  <si>
-    <t>弗雷尔卓德之心</t>
-  </si>
-  <si>
-    <t>戏命师</t>
-  </si>
-  <si>
-    <t>永猎双子</t>
-  </si>
-  <si>
-    <t>祖安花火</t>
-  </si>
-  <si>
-    <t>暴走萝莉</t>
-  </si>
-  <si>
-    <t>河流之王</t>
-  </si>
-  <si>
-    <t>破败之王</t>
-  </si>
-  <si>
-    <t>涤魂圣枪</t>
-  </si>
-  <si>
-    <t>影流之主</t>
-  </si>
-  <si>
-    <t>暴怒骑士</t>
-  </si>
-  <si>
-    <t>时间刺客</t>
-  </si>
-  <si>
-    <t>元素女皇</t>
-  </si>
-  <si>
-    <t>皮城执法官</t>
-  </si>
-  <si>
-    <t>暗裔剑魔</t>
-  </si>
-  <si>
-    <t>唤潮鲛姬</t>
-  </si>
-  <si>
-    <t>沙漠皇帝</t>
-  </si>
-  <si>
-    <t>魔法猫咪</t>
-  </si>
-  <si>
-    <t>沙漠玫瑰</t>
-  </si>
-  <si>
-    <t>魂锁典狱长</t>
-  </si>
-  <si>
-    <t>海兽祭司</t>
-  </si>
-  <si>
-    <t>虚空遁地兽</t>
-  </si>
-  <si>
-    <t>翠神</t>
-  </si>
-  <si>
-    <t>复仇之矛</t>
-  </si>
-  <si>
-    <t>星界游神</t>
-  </si>
-  <si>
-    <t>幻翎</t>
-  </si>
-  <si>
-    <t>逆羽</t>
-  </si>
-  <si>
-    <t>山隐之焰</t>
-  </si>
-  <si>
-    <t>解脱者</t>
-  </si>
-  <si>
-    <t>万花通灵</t>
-  </si>
-  <si>
-    <t>残月之肃</t>
-  </si>
-  <si>
-    <t>镕铁少女</t>
-  </si>
-  <si>
-    <t>血港鬼影</t>
-  </si>
-  <si>
-    <t>愁云使者</t>
-  </si>
-  <si>
-    <t>封魔剑魂</t>
-  </si>
-  <si>
-    <t>腕豪</t>
-  </si>
-  <si>
-    <t>含羞蓓蕾</t>
-  </si>
-  <si>
-    <t>灵罗娃娃</t>
-  </si>
-  <si>
-    <t>炼金男爵</t>
-  </si>
-  <si>
-    <t>Olaf</t>
-  </si>
-  <si>
-    <t>Twisted Fate</t>
-  </si>
-  <si>
-    <t>Xin Zhao</t>
-  </si>
-  <si>
-    <t>Urgot</t>
-  </si>
-  <si>
-    <t>Sion</t>
-  </si>
-  <si>
-    <t>Teemo</t>
-  </si>
-  <si>
-    <t>Cho'Gath</t>
-  </si>
-  <si>
-    <t>Anivia</t>
-  </si>
-  <si>
-    <t>Dr. Mundo</t>
-  </si>
-  <si>
-    <t>Sona</t>
-  </si>
-  <si>
-    <t>Kassadin</t>
-  </si>
-  <si>
-    <t>Irelia</t>
-  </si>
-  <si>
-    <t>Janna</t>
-  </si>
-  <si>
-    <t>Gangplank</t>
-  </si>
-  <si>
-    <t>Corki</t>
-  </si>
-  <si>
-    <t>Karma</t>
-  </si>
-  <si>
-    <t>Swain</t>
-  </si>
-  <si>
-    <t>Katarina</t>
-  </si>
-  <si>
-    <t>Nocturne</t>
-  </si>
-  <si>
-    <t>Maokai</t>
-  </si>
-  <si>
-    <t>Jarvan IV</t>
-  </si>
-  <si>
-    <t>Elise</t>
-  </si>
-  <si>
-    <t>Orianna</t>
-  </si>
-  <si>
-    <t>Lee Sin</t>
-  </si>
-  <si>
-    <t>Vayne</t>
-  </si>
-  <si>
-    <t>Rumble</t>
-  </si>
-  <si>
-    <t>Skarner</t>
-  </si>
-  <si>
-    <t>Heimerdinger</t>
-  </si>
-  <si>
-    <t>Poppy</t>
-  </si>
-  <si>
-    <t>Gragas</t>
-  </si>
-  <si>
-    <t>Pantheon</t>
-  </si>
-  <si>
-    <t>Mordekaiser</t>
-  </si>
-  <si>
-    <t>Yorick</t>
-  </si>
-  <si>
-    <t>Akali</t>
-  </si>
-  <si>
-    <t>Kennen</t>
-  </si>
-  <si>
-    <t>Malzahar</t>
-  </si>
-  <si>
-    <t>Talon</t>
-  </si>
-  <si>
-    <t>Riven</t>
-  </si>
-  <si>
-    <t>Kog'Maw</t>
-  </si>
-  <si>
-    <t>Xerath</t>
-  </si>
-  <si>
-    <t>Ahri</t>
-  </si>
-  <si>
-    <t>Fizz</t>
-  </si>
-  <si>
-    <t>Volibear</t>
-  </si>
-  <si>
-    <t>Rengar</t>
-  </si>
-  <si>
-    <t>Varus</t>
-  </si>
-  <si>
-    <t>Nautilus</t>
-  </si>
-  <si>
-    <t>Viktor</t>
-  </si>
-  <si>
-    <t>Sejuani</t>
-  </si>
-  <si>
-    <t>Fiora</t>
-  </si>
-  <si>
-    <t>Lulu</t>
-  </si>
-  <si>
-    <t>Draven</t>
-  </si>
-  <si>
-    <t>Hecarim</t>
-  </si>
-  <si>
-    <t>Jayce</t>
-  </si>
-  <si>
-    <t>Lissandra</t>
-  </si>
-  <si>
-    <t>Diana</t>
-  </si>
-  <si>
-    <t>Quinn</t>
-  </si>
-  <si>
-    <t>Syndra</t>
-  </si>
-  <si>
-    <t>Aurelion Sol</t>
-  </si>
-  <si>
-    <t>Kayn</t>
-  </si>
-  <si>
-    <t>Zoe</t>
-  </si>
-  <si>
-    <t>Kai'Sa</t>
-  </si>
-  <si>
-    <t>Seraphine</t>
-  </si>
-  <si>
-    <t>Gnar</t>
-  </si>
-  <si>
-    <t>Zac</t>
-  </si>
-  <si>
-    <t>Yasuo</t>
-  </si>
-  <si>
-    <t>Taliyah</t>
-  </si>
-  <si>
-    <t>Camille</t>
-  </si>
-  <si>
-    <t>Akshan</t>
-  </si>
-  <si>
-    <t>Braum</t>
-  </si>
-  <si>
-    <t>Jhin</t>
-  </si>
-  <si>
-    <t>Kindred</t>
-  </si>
-  <si>
-    <t>Zeri</t>
-  </si>
-  <si>
-    <t>Jinx</t>
-  </si>
-  <si>
-    <t>Tahm Kench</t>
-  </si>
-  <si>
-    <t>Viego</t>
-  </si>
-  <si>
-    <t>Senna</t>
-  </si>
-  <si>
-    <t>Zed</t>
-  </si>
-  <si>
-    <t>Kled</t>
-  </si>
-  <si>
-    <t>Ekko</t>
-  </si>
-  <si>
-    <t>Qiyana</t>
-  </si>
-  <si>
-    <t>Vi</t>
-  </si>
-  <si>
-    <t>Aatrox</t>
-  </si>
-  <si>
-    <t>Nami</t>
   </si>
   <si>
     <t>Azir</t>
@@ -1119,15 +994,9 @@
     <t>Khazix</t>
   </si>
   <si>
-    <t>Velkoz</t>
-  </si>
-  <si>
     <t>虚空女皇</t>
   </si>
   <si>
-    <t>Belveth</t>
-  </si>
-  <si>
     <t>不羁之悦</t>
   </si>
   <si>
@@ -1137,9 +1006,6 @@
     <t>纳祖芒荣耀</t>
   </si>
   <si>
-    <t>KSante</t>
-  </si>
-  <si>
     <t>明烛</t>
   </si>
   <si>
@@ -1152,12 +1018,31 @@
     <t>Naafiri</t>
   </si>
   <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>alias</t>
+  </si>
+  <si>
     <t>狂厄蔷薇</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Briar</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>异画师</t>
+  </si>
+  <si>
+    <t>Hwei</t>
+  </si>
+  <si>
+    <t>Vel'Koz</t>
+  </si>
+  <si>
+    <t>Bel'Veth</t>
+  </si>
+  <si>
+    <t>K'Sante</t>
   </si>
 </sst>
 </file>
@@ -1523,7 +1408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DF61A57-5822-4115-87D6-6E94EB78B234}">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1532,10 +1417,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>326</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1543,10 +1428,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1554,10 +1439,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1565,10 +1450,10 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1576,10 +1461,10 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1587,10 +1472,10 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1598,10 +1483,10 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1609,10 +1494,10 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1620,10 +1505,10 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1631,10 +1516,10 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1642,10 +1527,10 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1653,10 +1538,10 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1664,10 +1549,10 @@
         <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1675,10 +1560,10 @@
         <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1686,10 +1571,10 @@
         <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1697,10 +1582,10 @@
         <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1708,10 +1593,10 @@
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1719,10 +1604,10 @@
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1730,10 +1615,10 @@
         <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>92</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1741,10 +1626,10 @@
         <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1752,10 +1637,10 @@
         <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -1763,10 +1648,10 @@
         <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>93</v>
+        <v>216</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -1774,10 +1659,10 @@
         <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -1785,10 +1670,10 @@
         <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -1796,10 +1681,10 @@
         <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -1807,10 +1692,10 @@
         <v>51</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -1818,10 +1703,10 @@
         <v>53</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -1829,10 +1714,10 @@
         <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -1840,10 +1725,10 @@
         <v>58</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -1851,10 +1736,10 @@
         <v>62</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>316</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -1862,10 +1747,10 @@
         <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -1873,10 +1758,10 @@
         <v>69</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C32" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1884,10 +1769,10 @@
         <v>75</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C33" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -1895,10 +1780,10 @@
         <v>76</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C34" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -1906,10 +1791,10 @@
         <v>81</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C35" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -1917,10 +1802,10 @@
         <v>86</v>
       </c>
       <c r="B36" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C36" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -1928,10 +1813,10 @@
         <v>89</v>
       </c>
       <c r="B37" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C37" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -1939,10 +1824,10 @@
         <v>96</v>
       </c>
       <c r="B38" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C38" t="s">
-        <v>94</v>
+        <v>246</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -1950,10 +1835,10 @@
         <v>98</v>
       </c>
       <c r="B39" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C39" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -1961,10 +1846,10 @@
         <v>99</v>
       </c>
       <c r="B40" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C40" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -1972,10 +1857,10 @@
         <v>102</v>
       </c>
       <c r="B41" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C41" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -1983,10 +1868,10 @@
         <v>104</v>
       </c>
       <c r="B42" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C42" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -1994,10 +1879,10 @@
         <v>115</v>
       </c>
       <c r="B43" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C43" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -2005,10 +1890,10 @@
         <v>122</v>
       </c>
       <c r="B44" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C44" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -2016,10 +1901,10 @@
         <v>143</v>
       </c>
       <c r="B45" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C45" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -2027,10 +1912,10 @@
         <v>236</v>
       </c>
       <c r="B46" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C46" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2053,10 +1938,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>326</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2064,10 +1949,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2075,10 +1960,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>95</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2086,10 +1971,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2097,10 +1982,10 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2108,10 +1993,10 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2119,10 +2004,10 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2130,10 +2015,10 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2141,10 +2026,10 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2152,10 +2037,10 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C10" t="s">
-        <v>96</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2163,10 +2048,10 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -2174,10 +2059,10 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -2185,10 +2070,10 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="C13" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -2196,10 +2081,10 @@
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -2207,10 +2092,10 @@
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -2218,10 +2103,10 @@
         <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -2229,10 +2114,10 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -2240,10 +2125,10 @@
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -2251,10 +2136,10 @@
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -2262,10 +2147,10 @@
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -2273,10 +2158,10 @@
         <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -2284,10 +2169,10 @@
         <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>92</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -2295,10 +2180,10 @@
         <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -2306,10 +2191,10 @@
         <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -2317,10 +2202,10 @@
         <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>93</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -2328,10 +2213,10 @@
         <v>44</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -2339,10 +2224,10 @@
         <v>45</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -2350,10 +2235,10 @@
         <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C28" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -2361,10 +2246,10 @@
         <v>51</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -2372,10 +2257,10 @@
         <v>53</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -2383,10 +2268,10 @@
         <v>54</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C31" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -2394,10 +2279,10 @@
         <v>55</v>
       </c>
       <c r="B32" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C32" t="s">
-        <v>98</v>
+        <v>225</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -2405,10 +2290,10 @@
         <v>56</v>
       </c>
       <c r="B33" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="C33" t="s">
-        <v>99</v>
+        <v>226</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -2416,10 +2301,10 @@
         <v>58</v>
       </c>
       <c r="B34" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C34" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -2427,10 +2312,10 @@
         <v>61</v>
       </c>
       <c r="B35" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="C35" t="s">
-        <v>100</v>
+        <v>230</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -2438,10 +2323,10 @@
         <v>62</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C36" t="s">
-        <v>58</v>
+        <v>316</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -2449,10 +2334,10 @@
         <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C37" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -2460,10 +2345,10 @@
         <v>67</v>
       </c>
       <c r="B38" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="C38" t="s">
-        <v>101</v>
+        <v>232</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -2471,10 +2356,10 @@
         <v>69</v>
       </c>
       <c r="B39" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C39" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -2482,10 +2367,10 @@
         <v>74</v>
       </c>
       <c r="B40" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="C40" t="s">
-        <v>102</v>
+        <v>235</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -2493,10 +2378,10 @@
         <v>75</v>
       </c>
       <c r="B41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C41" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -2504,10 +2389,10 @@
         <v>76</v>
       </c>
       <c r="B42" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -2515,10 +2400,10 @@
         <v>81</v>
       </c>
       <c r="B43" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C43" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -2526,10 +2411,10 @@
         <v>86</v>
       </c>
       <c r="B44" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C44" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -2537,10 +2422,10 @@
         <v>89</v>
       </c>
       <c r="B45" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C45" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -2548,10 +2433,10 @@
         <v>90</v>
       </c>
       <c r="B46" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="C46" t="s">
-        <v>103</v>
+        <v>243</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -2559,10 +2444,10 @@
         <v>96</v>
       </c>
       <c r="B47" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C47" t="s">
-        <v>94</v>
+        <v>246</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -2570,10 +2455,10 @@
         <v>98</v>
       </c>
       <c r="B48" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C48" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -2581,10 +2466,10 @@
         <v>99</v>
       </c>
       <c r="B49" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C49" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -2592,10 +2477,10 @@
         <v>102</v>
       </c>
       <c r="B50" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C50" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -2603,10 +2488,10 @@
         <v>103</v>
       </c>
       <c r="B51" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="C51" t="s">
-        <v>104</v>
+        <v>248</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -2614,10 +2499,10 @@
         <v>104</v>
       </c>
       <c r="B52" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C52" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -2625,10 +2510,10 @@
         <v>115</v>
       </c>
       <c r="B53" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C53" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -2636,10 +2521,10 @@
         <v>117</v>
       </c>
       <c r="B54" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
       <c r="C54" t="s">
-        <v>105</v>
+        <v>257</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -2647,10 +2532,10 @@
         <v>122</v>
       </c>
       <c r="B55" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C55" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -2658,10 +2543,10 @@
         <v>143</v>
       </c>
       <c r="B56" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C56" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -2669,10 +2554,10 @@
         <v>222</v>
       </c>
       <c r="B57" t="s">
-        <v>118</v>
+        <v>174</v>
       </c>
       <c r="C57" t="s">
-        <v>106</v>
+        <v>280</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -2680,10 +2565,10 @@
         <v>236</v>
       </c>
       <c r="B58" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C58" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -2691,10 +2576,10 @@
         <v>267</v>
       </c>
       <c r="B59" t="s">
-        <v>119</v>
+        <v>184</v>
       </c>
       <c r="C59" t="s">
-        <v>107</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -2709,9 +2594,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94A1820C-C33D-44E8-9D81-D0A634174CBA}">
-  <dimension ref="A1:C166"/>
+  <dimension ref="A1:C167"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2720,10 +2605,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>326</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2731,10 +2616,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2742,10 +2627,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>240</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2753,10 +2638,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2764,10 +2649,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>136</v>
+        <v>104</v>
       </c>
       <c r="C5" t="s">
-        <v>241</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2775,10 +2660,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="C6" t="s">
-        <v>242</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2786,10 +2671,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
       <c r="C7" t="s">
-        <v>243</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2797,10 +2682,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
       <c r="C8" t="s">
-        <v>346</v>
+        <v>314</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2808,10 +2693,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2819,10 +2704,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>121</v>
+        <v>89</v>
       </c>
       <c r="C10" t="s">
-        <v>347</v>
+        <v>315</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2830,10 +2715,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -2841,10 +2726,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -2852,10 +2737,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -2863,10 +2748,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -2874,10 +2759,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>140</v>
+        <v>108</v>
       </c>
       <c r="C15" t="s">
-        <v>244</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -2885,10 +2770,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -2896,10 +2781,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -2907,10 +2792,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>141</v>
+        <v>109</v>
       </c>
       <c r="C18" t="s">
-        <v>245</v>
+        <v>213</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -2918,10 +2803,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -2929,10 +2814,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -2940,10 +2825,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>122</v>
+        <v>90</v>
       </c>
       <c r="C21" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -2951,10 +2836,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -2962,10 +2847,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -2973,10 +2858,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="C24" t="s">
-        <v>125</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -2984,10 +2869,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -2995,10 +2880,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -3006,10 +2891,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C27" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -3017,10 +2902,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
       <c r="C28" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -3028,10 +2913,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>131</v>
+        <v>99</v>
       </c>
       <c r="C29" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -3039,10 +2924,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="C30" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -3050,10 +2935,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -3061,10 +2946,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>246</v>
+        <v>214</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -3072,10 +2957,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -3083,10 +2968,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C34" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -3094,10 +2979,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="C35" t="s">
-        <v>247</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -3105,10 +2990,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>133</v>
+        <v>101</v>
       </c>
       <c r="C36" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -3116,10 +3001,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C37" t="s">
-        <v>248</v>
+        <v>216</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -3127,10 +3012,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>142</v>
+        <v>110</v>
       </c>
       <c r="C38" t="s">
-        <v>249</v>
+        <v>217</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -3138,10 +3023,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>143</v>
+        <v>111</v>
       </c>
       <c r="C39" t="s">
-        <v>250</v>
+        <v>218</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -3149,10 +3034,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>144</v>
+        <v>112</v>
       </c>
       <c r="C40" t="s">
-        <v>251</v>
+        <v>219</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -3160,10 +3045,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>145</v>
+        <v>113</v>
       </c>
       <c r="C41" t="s">
-        <v>252</v>
+        <v>220</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -3171,10 +3056,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="C42" t="s">
-        <v>253</v>
+        <v>221</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -3182,10 +3067,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>147</v>
+        <v>115</v>
       </c>
       <c r="C43" t="s">
-        <v>254</v>
+        <v>222</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -3193,10 +3078,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>148</v>
+        <v>116</v>
       </c>
       <c r="C44" t="s">
-        <v>255</v>
+        <v>223</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -3204,10 +3089,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C45" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -3215,10 +3100,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C46" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -3226,10 +3111,10 @@
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -3237,10 +3122,10 @@
         <v>50</v>
       </c>
       <c r="B48" t="s">
-        <v>149</v>
+        <v>117</v>
       </c>
       <c r="C48" t="s">
-        <v>256</v>
+        <v>224</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -3248,10 +3133,10 @@
         <v>51</v>
       </c>
       <c r="B49" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C49" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -3259,10 +3144,10 @@
         <v>53</v>
       </c>
       <c r="B50" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C50" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -3270,10 +3155,10 @@
         <v>54</v>
       </c>
       <c r="B51" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C51" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -3281,10 +3166,10 @@
         <v>55</v>
       </c>
       <c r="B52" t="s">
-        <v>150</v>
+        <v>118</v>
       </c>
       <c r="C52" t="s">
-        <v>257</v>
+        <v>225</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -3292,10 +3177,10 @@
         <v>56</v>
       </c>
       <c r="B53" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
       <c r="C53" t="s">
-        <v>258</v>
+        <v>226</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -3303,10 +3188,10 @@
         <v>57</v>
       </c>
       <c r="B54" t="s">
-        <v>152</v>
+        <v>120</v>
       </c>
       <c r="C54" t="s">
-        <v>259</v>
+        <v>227</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -3314,10 +3199,10 @@
         <v>58</v>
       </c>
       <c r="B55" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C55" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -3325,10 +3210,10 @@
         <v>59</v>
       </c>
       <c r="B56" t="s">
-        <v>153</v>
+        <v>121</v>
       </c>
       <c r="C56" t="s">
-        <v>260</v>
+        <v>228</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -3336,10 +3221,10 @@
         <v>60</v>
       </c>
       <c r="B57" t="s">
-        <v>154</v>
+        <v>122</v>
       </c>
       <c r="C57" t="s">
-        <v>261</v>
+        <v>229</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -3347,10 +3232,10 @@
         <v>61</v>
       </c>
       <c r="B58" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C58" t="s">
-        <v>262</v>
+        <v>230</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -3358,10 +3243,10 @@
         <v>62</v>
       </c>
       <c r="B59" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C59" t="s">
-        <v>348</v>
+        <v>316</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -3369,10 +3254,10 @@
         <v>63</v>
       </c>
       <c r="B60" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C60" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -3380,10 +3265,10 @@
         <v>64</v>
       </c>
       <c r="B61" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="C61" t="s">
-        <v>263</v>
+        <v>231</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -3391,10 +3276,10 @@
         <v>67</v>
       </c>
       <c r="B62" t="s">
-        <v>157</v>
+        <v>125</v>
       </c>
       <c r="C62" t="s">
-        <v>264</v>
+        <v>232</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -3402,10 +3287,10 @@
         <v>68</v>
       </c>
       <c r="B63" t="s">
-        <v>158</v>
+        <v>126</v>
       </c>
       <c r="C63" t="s">
-        <v>265</v>
+        <v>233</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -3413,10 +3298,10 @@
         <v>69</v>
       </c>
       <c r="B64" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C64" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -3424,10 +3309,10 @@
         <v>72</v>
       </c>
       <c r="B65" t="s">
-        <v>159</v>
+        <v>127</v>
       </c>
       <c r="C65" t="s">
-        <v>266</v>
+        <v>234</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -3435,10 +3320,10 @@
         <v>74</v>
       </c>
       <c r="B66" t="s">
-        <v>160</v>
+        <v>128</v>
       </c>
       <c r="C66" t="s">
-        <v>267</v>
+        <v>235</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -3446,10 +3331,10 @@
         <v>75</v>
       </c>
       <c r="B67" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C67" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -3457,10 +3342,10 @@
         <v>76</v>
       </c>
       <c r="B68" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C68" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -3468,10 +3353,10 @@
         <v>77</v>
       </c>
       <c r="B69" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C69" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -3479,10 +3364,10 @@
         <v>78</v>
       </c>
       <c r="B70" t="s">
-        <v>161</v>
+        <v>129</v>
       </c>
       <c r="C70" t="s">
-        <v>268</v>
+        <v>236</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -3490,10 +3375,10 @@
         <v>79</v>
       </c>
       <c r="B71" t="s">
-        <v>162</v>
+        <v>130</v>
       </c>
       <c r="C71" t="s">
-        <v>269</v>
+        <v>237</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -3501,10 +3386,10 @@
         <v>80</v>
       </c>
       <c r="B72" t="s">
-        <v>163</v>
+        <v>131</v>
       </c>
       <c r="C72" t="s">
-        <v>270</v>
+        <v>238</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -3512,10 +3397,10 @@
         <v>81</v>
       </c>
       <c r="B73" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C73" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -3523,10 +3408,10 @@
         <v>82</v>
       </c>
       <c r="B74" t="s">
-        <v>164</v>
+        <v>132</v>
       </c>
       <c r="C74" t="s">
-        <v>271</v>
+        <v>239</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -3534,10 +3419,10 @@
         <v>83</v>
       </c>
       <c r="B75" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="C75" t="s">
-        <v>272</v>
+        <v>240</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -3545,10 +3430,10 @@
         <v>84</v>
       </c>
       <c r="B76" t="s">
-        <v>166</v>
+        <v>134</v>
       </c>
       <c r="C76" t="s">
-        <v>273</v>
+        <v>241</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -3556,10 +3441,10 @@
         <v>85</v>
       </c>
       <c r="B77" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="C77" t="s">
-        <v>274</v>
+        <v>242</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -3567,10 +3452,10 @@
         <v>86</v>
       </c>
       <c r="B78" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C78" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -3578,10 +3463,10 @@
         <v>89</v>
       </c>
       <c r="B79" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C79" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -3589,10 +3474,10 @@
         <v>90</v>
       </c>
       <c r="B80" t="s">
-        <v>168</v>
+        <v>136</v>
       </c>
       <c r="C80" t="s">
-        <v>275</v>
+        <v>243</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -3600,10 +3485,10 @@
         <v>91</v>
       </c>
       <c r="B81" t="s">
-        <v>169</v>
+        <v>137</v>
       </c>
       <c r="C81" t="s">
-        <v>276</v>
+        <v>244</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -3611,10 +3496,10 @@
         <v>92</v>
       </c>
       <c r="B82" t="s">
-        <v>170</v>
+        <v>138</v>
       </c>
       <c r="C82" t="s">
-        <v>277</v>
+        <v>245</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -3622,10 +3507,10 @@
         <v>96</v>
       </c>
       <c r="B83" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C83" t="s">
-        <v>278</v>
+        <v>246</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -3633,10 +3518,10 @@
         <v>98</v>
       </c>
       <c r="B84" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C84" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -3644,10 +3529,10 @@
         <v>99</v>
       </c>
       <c r="B85" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C85" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -3655,10 +3540,10 @@
         <v>101</v>
       </c>
       <c r="B86" t="s">
-        <v>171</v>
+        <v>139</v>
       </c>
       <c r="C86" t="s">
-        <v>279</v>
+        <v>247</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -3666,10 +3551,10 @@
         <v>102</v>
       </c>
       <c r="B87" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C87" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -3677,10 +3562,10 @@
         <v>103</v>
       </c>
       <c r="B88" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
       <c r="C88" t="s">
-        <v>280</v>
+        <v>248</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -3688,10 +3573,10 @@
         <v>104</v>
       </c>
       <c r="B89" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C89" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -3699,10 +3584,10 @@
         <v>105</v>
       </c>
       <c r="B90" t="s">
-        <v>173</v>
+        <v>141</v>
       </c>
       <c r="C90" t="s">
-        <v>281</v>
+        <v>249</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -3710,10 +3595,10 @@
         <v>106</v>
       </c>
       <c r="B91" t="s">
-        <v>174</v>
+        <v>142</v>
       </c>
       <c r="C91" t="s">
-        <v>282</v>
+        <v>250</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -3721,10 +3606,10 @@
         <v>107</v>
       </c>
       <c r="B92" t="s">
-        <v>175</v>
+        <v>143</v>
       </c>
       <c r="C92" t="s">
-        <v>283</v>
+        <v>251</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -3732,10 +3617,10 @@
         <v>110</v>
       </c>
       <c r="B93" t="s">
-        <v>176</v>
+        <v>144</v>
       </c>
       <c r="C93" t="s">
-        <v>284</v>
+        <v>252</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -3743,10 +3628,10 @@
         <v>111</v>
       </c>
       <c r="B94" t="s">
-        <v>177</v>
+        <v>145</v>
       </c>
       <c r="C94" t="s">
-        <v>285</v>
+        <v>253</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -3754,10 +3639,10 @@
         <v>112</v>
       </c>
       <c r="B95" t="s">
-        <v>178</v>
+        <v>146</v>
       </c>
       <c r="C95" t="s">
-        <v>286</v>
+        <v>254</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -3765,10 +3650,10 @@
         <v>113</v>
       </c>
       <c r="B96" t="s">
-        <v>179</v>
+        <v>147</v>
       </c>
       <c r="C96" t="s">
-        <v>287</v>
+        <v>255</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -3776,10 +3661,10 @@
         <v>114</v>
       </c>
       <c r="B97" t="s">
-        <v>180</v>
+        <v>148</v>
       </c>
       <c r="C97" t="s">
-        <v>288</v>
+        <v>256</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -3787,10 +3672,10 @@
         <v>115</v>
       </c>
       <c r="B98" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C98" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -3798,10 +3683,10 @@
         <v>117</v>
       </c>
       <c r="B99" t="s">
-        <v>181</v>
+        <v>149</v>
       </c>
       <c r="C99" t="s">
-        <v>289</v>
+        <v>257</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -3809,10 +3694,10 @@
         <v>119</v>
       </c>
       <c r="B100" t="s">
-        <v>182</v>
+        <v>150</v>
       </c>
       <c r="C100" t="s">
-        <v>290</v>
+        <v>258</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -3820,10 +3705,10 @@
         <v>120</v>
       </c>
       <c r="B101" t="s">
-        <v>183</v>
+        <v>151</v>
       </c>
       <c r="C101" t="s">
-        <v>291</v>
+        <v>259</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -3831,10 +3716,10 @@
         <v>121</v>
       </c>
       <c r="B102" t="s">
-        <v>184</v>
+        <v>152</v>
       </c>
       <c r="C102" t="s">
-        <v>349</v>
+        <v>317</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -3842,10 +3727,10 @@
         <v>122</v>
       </c>
       <c r="B103" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C103" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -3853,10 +3738,10 @@
         <v>126</v>
       </c>
       <c r="B104" t="s">
-        <v>185</v>
+        <v>153</v>
       </c>
       <c r="C104" t="s">
-        <v>292</v>
+        <v>260</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -3864,10 +3749,10 @@
         <v>127</v>
       </c>
       <c r="B105" t="s">
-        <v>186</v>
+        <v>154</v>
       </c>
       <c r="C105" t="s">
-        <v>293</v>
+        <v>261</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -3875,10 +3760,10 @@
         <v>131</v>
       </c>
       <c r="B106" t="s">
-        <v>187</v>
+        <v>155</v>
       </c>
       <c r="C106" t="s">
-        <v>294</v>
+        <v>262</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -3886,10 +3771,10 @@
         <v>133</v>
       </c>
       <c r="B107" t="s">
-        <v>188</v>
+        <v>156</v>
       </c>
       <c r="C107" t="s">
-        <v>295</v>
+        <v>263</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -3897,10 +3782,10 @@
         <v>134</v>
       </c>
       <c r="B108" t="s">
-        <v>189</v>
+        <v>157</v>
       </c>
       <c r="C108" t="s">
-        <v>296</v>
+        <v>264</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -3908,10 +3793,10 @@
         <v>136</v>
       </c>
       <c r="B109" t="s">
-        <v>190</v>
+        <v>158</v>
       </c>
       <c r="C109" t="s">
-        <v>297</v>
+        <v>265</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -3919,10 +3804,10 @@
         <v>141</v>
       </c>
       <c r="B110" t="s">
-        <v>191</v>
+        <v>159</v>
       </c>
       <c r="C110" t="s">
-        <v>298</v>
+        <v>266</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -3930,10 +3815,10 @@
         <v>142</v>
       </c>
       <c r="B111" t="s">
-        <v>192</v>
+        <v>160</v>
       </c>
       <c r="C111" t="s">
-        <v>299</v>
+        <v>267</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -3941,10 +3826,10 @@
         <v>143</v>
       </c>
       <c r="B112" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C112" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -3952,10 +3837,10 @@
         <v>145</v>
       </c>
       <c r="B113" t="s">
-        <v>193</v>
+        <v>161</v>
       </c>
       <c r="C113" t="s">
-        <v>300</v>
+        <v>268</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -3963,10 +3848,10 @@
         <v>147</v>
       </c>
       <c r="B114" t="s">
-        <v>194</v>
+        <v>162</v>
       </c>
       <c r="C114" t="s">
-        <v>301</v>
+        <v>269</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -3974,10 +3859,10 @@
         <v>150</v>
       </c>
       <c r="B115" t="s">
-        <v>195</v>
+        <v>163</v>
       </c>
       <c r="C115" t="s">
-        <v>302</v>
+        <v>270</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -3985,10 +3870,10 @@
         <v>154</v>
       </c>
       <c r="B116" t="s">
-        <v>196</v>
+        <v>164</v>
       </c>
       <c r="C116" t="s">
-        <v>303</v>
+        <v>271</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -3996,10 +3881,10 @@
         <v>157</v>
       </c>
       <c r="B117" t="s">
-        <v>197</v>
+        <v>165</v>
       </c>
       <c r="C117" t="s">
-        <v>304</v>
+        <v>272</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -4007,10 +3892,10 @@
         <v>161</v>
       </c>
       <c r="B118" t="s">
-        <v>198</v>
+        <v>166</v>
       </c>
       <c r="C118" t="s">
-        <v>350</v>
+        <v>332</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -4018,10 +3903,10 @@
         <v>163</v>
       </c>
       <c r="B119" t="s">
-        <v>199</v>
+        <v>167</v>
       </c>
       <c r="C119" t="s">
-        <v>305</v>
+        <v>273</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -4029,10 +3914,10 @@
         <v>164</v>
       </c>
       <c r="B120" t="s">
-        <v>200</v>
+        <v>168</v>
       </c>
       <c r="C120" t="s">
-        <v>306</v>
+        <v>274</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -4040,10 +3925,10 @@
         <v>166</v>
       </c>
       <c r="B121" t="s">
-        <v>201</v>
+        <v>169</v>
       </c>
       <c r="C121" t="s">
-        <v>307</v>
+        <v>275</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
@@ -4051,10 +3936,10 @@
         <v>200</v>
       </c>
       <c r="B122" t="s">
-        <v>351</v>
+        <v>318</v>
       </c>
       <c r="C122" t="s">
-        <v>352</v>
+        <v>333</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
@@ -4062,10 +3947,10 @@
         <v>201</v>
       </c>
       <c r="B123" t="s">
-        <v>202</v>
+        <v>170</v>
       </c>
       <c r="C123" t="s">
-        <v>308</v>
+        <v>276</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
@@ -4073,10 +3958,10 @@
         <v>202</v>
       </c>
       <c r="B124" t="s">
-        <v>203</v>
+        <v>171</v>
       </c>
       <c r="C124" t="s">
-        <v>309</v>
+        <v>277</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
@@ -4084,10 +3969,10 @@
         <v>203</v>
       </c>
       <c r="B125" t="s">
-        <v>204</v>
+        <v>172</v>
       </c>
       <c r="C125" t="s">
-        <v>310</v>
+        <v>278</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
@@ -4095,10 +3980,10 @@
         <v>221</v>
       </c>
       <c r="B126" t="s">
-        <v>205</v>
+        <v>173</v>
       </c>
       <c r="C126" t="s">
-        <v>311</v>
+        <v>279</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
@@ -4106,10 +3991,10 @@
         <v>222</v>
       </c>
       <c r="B127" t="s">
-        <v>206</v>
+        <v>174</v>
       </c>
       <c r="C127" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
@@ -4117,10 +4002,10 @@
         <v>223</v>
       </c>
       <c r="B128" t="s">
-        <v>207</v>
+        <v>175</v>
       </c>
       <c r="C128" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
@@ -4128,10 +4013,10 @@
         <v>233</v>
       </c>
       <c r="B129" t="s">
-        <v>361</v>
+        <v>328</v>
       </c>
       <c r="C129" t="s">
-        <v>362</v>
+        <v>329</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
@@ -4139,10 +4024,10 @@
         <v>234</v>
       </c>
       <c r="B130" t="s">
-        <v>208</v>
+        <v>176</v>
       </c>
       <c r="C130" t="s">
-        <v>314</v>
+        <v>282</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
@@ -4150,10 +4035,10 @@
         <v>235</v>
       </c>
       <c r="B131" t="s">
-        <v>209</v>
+        <v>177</v>
       </c>
       <c r="C131" t="s">
-        <v>315</v>
+        <v>283</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
@@ -4161,10 +4046,10 @@
         <v>236</v>
       </c>
       <c r="B132" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C132" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
@@ -4172,10 +4057,10 @@
         <v>238</v>
       </c>
       <c r="B133" t="s">
-        <v>210</v>
+        <v>178</v>
       </c>
       <c r="C133" t="s">
-        <v>316</v>
+        <v>284</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
@@ -4183,10 +4068,10 @@
         <v>240</v>
       </c>
       <c r="B134" t="s">
-        <v>211</v>
+        <v>179</v>
       </c>
       <c r="C134" t="s">
-        <v>317</v>
+        <v>285</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
@@ -4194,10 +4079,10 @@
         <v>245</v>
       </c>
       <c r="B135" t="s">
-        <v>212</v>
+        <v>180</v>
       </c>
       <c r="C135" t="s">
-        <v>318</v>
+        <v>286</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
@@ -4205,10 +4090,10 @@
         <v>246</v>
       </c>
       <c r="B136" t="s">
-        <v>213</v>
+        <v>181</v>
       </c>
       <c r="C136" t="s">
-        <v>319</v>
+        <v>287</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
@@ -4216,10 +4101,10 @@
         <v>254</v>
       </c>
       <c r="B137" t="s">
-        <v>214</v>
+        <v>182</v>
       </c>
       <c r="C137" t="s">
-        <v>320</v>
+        <v>288</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
@@ -4227,10 +4112,10 @@
         <v>266</v>
       </c>
       <c r="B138" t="s">
-        <v>215</v>
+        <v>183</v>
       </c>
       <c r="C138" t="s">
-        <v>321</v>
+        <v>289</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
@@ -4238,10 +4123,10 @@
         <v>267</v>
       </c>
       <c r="B139" t="s">
-        <v>216</v>
+        <v>184</v>
       </c>
       <c r="C139" t="s">
-        <v>322</v>
+        <v>290</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
@@ -4249,10 +4134,10 @@
         <v>268</v>
       </c>
       <c r="B140" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
       <c r="C140" t="s">
-        <v>323</v>
+        <v>291</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
@@ -4260,10 +4145,10 @@
         <v>350</v>
       </c>
       <c r="B141" t="s">
-        <v>218</v>
+        <v>186</v>
       </c>
       <c r="C141" t="s">
-        <v>324</v>
+        <v>292</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
@@ -4271,10 +4156,10 @@
         <v>360</v>
       </c>
       <c r="B142" t="s">
-        <v>219</v>
+        <v>187</v>
       </c>
       <c r="C142" t="s">
-        <v>325</v>
+        <v>293</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
@@ -4282,10 +4167,10 @@
         <v>412</v>
       </c>
       <c r="B143" t="s">
-        <v>220</v>
+        <v>188</v>
       </c>
       <c r="C143" t="s">
-        <v>326</v>
+        <v>294</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
@@ -4293,10 +4178,10 @@
         <v>420</v>
       </c>
       <c r="B144" t="s">
-        <v>221</v>
+        <v>189</v>
       </c>
       <c r="C144" t="s">
-        <v>327</v>
+        <v>295</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
@@ -4304,10 +4189,10 @@
         <v>421</v>
       </c>
       <c r="B145" t="s">
-        <v>222</v>
+        <v>190</v>
       </c>
       <c r="C145" t="s">
-        <v>328</v>
+        <v>296</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
@@ -4315,10 +4200,10 @@
         <v>427</v>
       </c>
       <c r="B146" t="s">
-        <v>223</v>
+        <v>191</v>
       </c>
       <c r="C146" t="s">
-        <v>329</v>
+        <v>297</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
@@ -4326,10 +4211,10 @@
         <v>429</v>
       </c>
       <c r="B147" t="s">
-        <v>224</v>
+        <v>192</v>
       </c>
       <c r="C147" t="s">
-        <v>330</v>
+        <v>298</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
@@ -4337,10 +4222,10 @@
         <v>432</v>
       </c>
       <c r="B148" t="s">
-        <v>225</v>
+        <v>193</v>
       </c>
       <c r="C148" t="s">
-        <v>331</v>
+        <v>299</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
@@ -4348,10 +4233,10 @@
         <v>497</v>
       </c>
       <c r="B149" t="s">
-        <v>226</v>
+        <v>194</v>
       </c>
       <c r="C149" t="s">
-        <v>332</v>
+        <v>300</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
@@ -4359,10 +4244,10 @@
         <v>498</v>
       </c>
       <c r="B150" t="s">
-        <v>227</v>
+        <v>195</v>
       </c>
       <c r="C150" t="s">
-        <v>333</v>
+        <v>301</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
@@ -4370,10 +4255,10 @@
         <v>516</v>
       </c>
       <c r="B151" t="s">
-        <v>228</v>
+        <v>196</v>
       </c>
       <c r="C151" t="s">
-        <v>334</v>
+        <v>302</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
@@ -4381,10 +4266,10 @@
         <v>517</v>
       </c>
       <c r="B152" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
       <c r="C152" t="s">
-        <v>335</v>
+        <v>303</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
@@ -4392,10 +4277,10 @@
         <v>518</v>
       </c>
       <c r="B153" t="s">
-        <v>230</v>
+        <v>198</v>
       </c>
       <c r="C153" t="s">
-        <v>336</v>
+        <v>304</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
@@ -4403,10 +4288,10 @@
         <v>523</v>
       </c>
       <c r="B154" t="s">
-        <v>231</v>
+        <v>199</v>
       </c>
       <c r="C154" t="s">
-        <v>337</v>
+        <v>305</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
@@ -4414,10 +4299,10 @@
         <v>526</v>
       </c>
       <c r="B155" t="s">
-        <v>232</v>
+        <v>200</v>
       </c>
       <c r="C155" t="s">
-        <v>338</v>
+        <v>306</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
@@ -4425,10 +4310,10 @@
         <v>555</v>
       </c>
       <c r="B156" t="s">
-        <v>233</v>
+        <v>201</v>
       </c>
       <c r="C156" t="s">
-        <v>339</v>
+        <v>307</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
@@ -4436,10 +4321,10 @@
         <v>711</v>
       </c>
       <c r="B157" t="s">
-        <v>234</v>
+        <v>202</v>
       </c>
       <c r="C157" t="s">
-        <v>340</v>
+        <v>308</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
@@ -4447,10 +4332,10 @@
         <v>777</v>
       </c>
       <c r="B158" t="s">
-        <v>235</v>
+        <v>203</v>
       </c>
       <c r="C158" t="s">
-        <v>341</v>
+        <v>309</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
@@ -4458,10 +4343,10 @@
         <v>875</v>
       </c>
       <c r="B159" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
       <c r="C159" t="s">
-        <v>342</v>
+        <v>310</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
@@ -4469,10 +4354,10 @@
         <v>876</v>
       </c>
       <c r="B160" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
       <c r="C160" t="s">
-        <v>343</v>
+        <v>311</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
@@ -4480,10 +4365,10 @@
         <v>887</v>
       </c>
       <c r="B161" t="s">
-        <v>238</v>
+        <v>206</v>
       </c>
       <c r="C161" t="s">
-        <v>344</v>
+        <v>312</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
@@ -4491,10 +4376,10 @@
         <v>888</v>
       </c>
       <c r="B162" t="s">
-        <v>239</v>
+        <v>207</v>
       </c>
       <c r="C162" t="s">
-        <v>345</v>
+        <v>313</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
@@ -4502,10 +4387,10 @@
         <v>895</v>
       </c>
       <c r="B163" t="s">
-        <v>353</v>
+        <v>319</v>
       </c>
       <c r="C163" t="s">
-        <v>354</v>
+        <v>320</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
@@ -4513,10 +4398,10 @@
         <v>897</v>
       </c>
       <c r="B164" t="s">
-        <v>355</v>
+        <v>321</v>
       </c>
       <c r="C164" t="s">
-        <v>356</v>
+        <v>334</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
@@ -4524,21 +4409,32 @@
         <v>902</v>
       </c>
       <c r="B165" t="s">
-        <v>357</v>
+        <v>322</v>
       </c>
       <c r="C165" t="s">
-        <v>358</v>
+        <v>323</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166">
+        <v>910</v>
+      </c>
+      <c r="B166" t="s">
+        <v>330</v>
+      </c>
+      <c r="C166" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A167">
         <v>950</v>
       </c>
-      <c r="B166" t="s">
-        <v>359</v>
-      </c>
-      <c r="C166" t="s">
-        <v>360</v>
+      <c r="B167" t="s">
+        <v>324</v>
+      </c>
+      <c r="C167" t="s">
+        <v>325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
自定义脚本11的一个品质级改动【An Quality Update of Customized Program 11】
现在，自定义脚本11允许切换模式了。如果感兴趣的话，请自行探索程序的哪些阶段允许切换模式。
Now, mode switching is enabled in Customized Program 11. If you're interested, please explore the stages that allows mode switching during the program execution by yourself.
另外，更新了离线数据资源文件。（最近更新：2024年3月15日。）
Besides, updated offline data resources. (Latest update: 2024-03-15.)
</commit_message>
<xml_diff>
--- a/available-bots.xlsx
+++ b/available-bots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19250\Documents\GitHub\LoL-DIY-Programs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9E02C1-CF36-4B69-A594-EC7D4F2D6712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58840920-0442-4B80-994E-A652E236E095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{79371658-E0FE-43C3-8A19-9910316D4D47}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="337">
   <si>
     <t>championId</t>
   </si>
@@ -1933,7 +1933,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C1DA04B-86DE-4C1C-948C-D98ADF48BF05}">
-  <dimension ref="A1:C59"/>
+  <dimension ref="A1:C94"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1985,607 +1985,992 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>104</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>105</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>108</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>212</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>109</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>213</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
         <v>18</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
         <v>22</v>
-      </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
         <v>24</v>
-      </c>
-      <c r="B18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
         <v>25</v>
       </c>
-      <c r="B19" t="s">
-        <v>29</v>
-      </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>214</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
         <v>32</v>
-      </c>
-      <c r="B23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>216</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C26" t="s">
-        <v>42</v>
+        <v>214</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>216</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>110</v>
       </c>
       <c r="C30" t="s">
-        <v>50</v>
+        <v>217</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
+        <v>111</v>
       </c>
       <c r="C31" t="s">
-        <v>52</v>
+        <v>218</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="B32" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C32" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B33" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C33" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B35" t="s">
-        <v>123</v>
+        <v>43</v>
       </c>
       <c r="C35" t="s">
-        <v>230</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C36" t="s">
-        <v>316</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B37" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C37" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="B38" t="s">
-        <v>125</v>
+        <v>49</v>
       </c>
       <c r="C38" t="s">
-        <v>232</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B39" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C39" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="B40" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C40" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="B41" t="s">
-        <v>60</v>
+        <v>119</v>
       </c>
       <c r="C41" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="B42" t="s">
-        <v>62</v>
+        <v>120</v>
       </c>
       <c r="C42" t="s">
-        <v>63</v>
+        <v>227</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="B43" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C43" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="B44" t="s">
-        <v>68</v>
+        <v>123</v>
       </c>
       <c r="C44" t="s">
-        <v>69</v>
+        <v>230</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="B45" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C45" t="s">
-        <v>71</v>
+        <v>316</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="B46" t="s">
-        <v>136</v>
+        <v>56</v>
       </c>
       <c r="C46" t="s">
-        <v>243</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="B47" t="s">
-        <v>72</v>
+        <v>125</v>
       </c>
       <c r="C47" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="B48" t="s">
-        <v>73</v>
+        <v>126</v>
       </c>
       <c r="C48" t="s">
-        <v>74</v>
+        <v>233</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="B49" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="C49" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="B50" t="s">
-        <v>77</v>
+        <v>128</v>
       </c>
       <c r="C50" t="s">
-        <v>78</v>
+        <v>235</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="B51" t="s">
-        <v>140</v>
+        <v>60</v>
       </c>
       <c r="C51" t="s">
-        <v>248</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="B52" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="C52" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>115</v>
+        <v>78</v>
       </c>
       <c r="B53" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
       <c r="C53" t="s">
-        <v>82</v>
+        <v>236</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>117</v>
+        <v>81</v>
       </c>
       <c r="B54" t="s">
-        <v>149</v>
+        <v>66</v>
       </c>
       <c r="C54" t="s">
-        <v>257</v>
+        <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="B55" t="s">
-        <v>83</v>
+        <v>132</v>
       </c>
       <c r="C55" t="s">
-        <v>84</v>
+        <v>239</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>143</v>
+        <v>83</v>
       </c>
       <c r="B56" t="s">
-        <v>85</v>
+        <v>133</v>
       </c>
       <c r="C56" t="s">
-        <v>86</v>
+        <v>240</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>222</v>
+        <v>84</v>
       </c>
       <c r="B57" t="s">
-        <v>174</v>
+        <v>134</v>
       </c>
       <c r="C57" t="s">
-        <v>280</v>
+        <v>241</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>236</v>
+        <v>85</v>
       </c>
       <c r="B58" t="s">
-        <v>87</v>
+        <v>135</v>
       </c>
       <c r="C58" t="s">
-        <v>88</v>
+        <v>242</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>267</v>
+        <v>86</v>
       </c>
       <c r="B59" t="s">
-        <v>184</v>
+        <v>68</v>
       </c>
       <c r="C59" t="s">
-        <v>290</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>89</v>
+      </c>
+      <c r="B60" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>90</v>
+      </c>
+      <c r="B61" t="s">
+        <v>136</v>
+      </c>
+      <c r="C61" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>96</v>
+      </c>
+      <c r="B62" t="s">
+        <v>72</v>
+      </c>
+      <c r="C62" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>98</v>
+      </c>
+      <c r="B63" t="s">
+        <v>73</v>
+      </c>
+      <c r="C63" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>99</v>
+      </c>
+      <c r="B64" t="s">
+        <v>75</v>
+      </c>
+      <c r="C64" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>102</v>
+      </c>
+      <c r="B65" t="s">
+        <v>77</v>
+      </c>
+      <c r="C65" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>103</v>
+      </c>
+      <c r="B66" t="s">
+        <v>140</v>
+      </c>
+      <c r="C66" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>104</v>
+      </c>
+      <c r="B67" t="s">
+        <v>79</v>
+      </c>
+      <c r="C67" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>105</v>
+      </c>
+      <c r="B68" t="s">
+        <v>141</v>
+      </c>
+      <c r="C68" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>106</v>
+      </c>
+      <c r="B69" t="s">
+        <v>142</v>
+      </c>
+      <c r="C69" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>110</v>
+      </c>
+      <c r="B70" t="s">
+        <v>144</v>
+      </c>
+      <c r="C70" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>111</v>
+      </c>
+      <c r="B71" t="s">
+        <v>145</v>
+      </c>
+      <c r="C71" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>112</v>
+      </c>
+      <c r="B72" t="s">
+        <v>146</v>
+      </c>
+      <c r="C72" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>113</v>
+      </c>
+      <c r="B73" t="s">
+        <v>147</v>
+      </c>
+      <c r="C73" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>115</v>
+      </c>
+      <c r="B74" t="s">
+        <v>81</v>
+      </c>
+      <c r="C74" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>117</v>
+      </c>
+      <c r="B75" t="s">
+        <v>149</v>
+      </c>
+      <c r="C75" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>120</v>
+      </c>
+      <c r="B76" t="s">
+        <v>151</v>
+      </c>
+      <c r="C76" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>121</v>
+      </c>
+      <c r="B77" t="s">
+        <v>152</v>
+      </c>
+      <c r="C77" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>122</v>
+      </c>
+      <c r="B78" t="s">
+        <v>83</v>
+      </c>
+      <c r="C78" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>127</v>
+      </c>
+      <c r="B79" t="s">
+        <v>154</v>
+      </c>
+      <c r="C79" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>131</v>
+      </c>
+      <c r="B80" t="s">
+        <v>155</v>
+      </c>
+      <c r="C80" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>143</v>
+      </c>
+      <c r="B81" t="s">
+        <v>85</v>
+      </c>
+      <c r="C81" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>145</v>
+      </c>
+      <c r="B82" t="s">
+        <v>161</v>
+      </c>
+      <c r="C82" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>147</v>
+      </c>
+      <c r="B83" t="s">
+        <v>162</v>
+      </c>
+      <c r="C83" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>201</v>
+      </c>
+      <c r="B84" t="s">
+        <v>170</v>
+      </c>
+      <c r="C84" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>236</v>
+      </c>
+      <c r="B85" t="s">
+        <v>87</v>
+      </c>
+      <c r="C85" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>254</v>
+      </c>
+      <c r="B86" t="s">
+        <v>182</v>
+      </c>
+      <c r="C86" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>266</v>
+      </c>
+      <c r="B87" t="s">
+        <v>183</v>
+      </c>
+      <c r="C87" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>497</v>
+      </c>
+      <c r="B88" t="s">
+        <v>194</v>
+      </c>
+      <c r="C88" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>711</v>
+      </c>
+      <c r="B89" t="s">
+        <v>202</v>
+      </c>
+      <c r="C89" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>875</v>
+      </c>
+      <c r="B90" t="s">
+        <v>204</v>
+      </c>
+      <c r="C90" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>876</v>
+      </c>
+      <c r="B91" t="s">
+        <v>205</v>
+      </c>
+      <c r="C91" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>888</v>
+      </c>
+      <c r="B92" t="s">
+        <v>207</v>
+      </c>
+      <c r="C92" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>901</v>
+      </c>
+      <c r="B93" t="s">
+        <v>335</v>
+      </c>
+      <c r="C93" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>902</v>
+      </c>
+      <c r="B94" t="s">
+        <v>322</v>
+      </c>
+      <c r="C94" t="s">
+        <v>323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>